<commit_message>
Tvchannels toaster message updated for all the test case
</commit_message>
<xml_diff>
--- a/Elevate20/src/main/java/io/stage/hudinielevate/cms/testdata/TestData.xlsx
+++ b/Elevate20/src/main/java/io/stage/hudinielevate/cms/testdata/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6920" activeTab="6"/>
+    <workbookView windowWidth="1000" windowHeight="450" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Group" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="ActivityCalendar" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <oleSize ref="A1:O3"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1211,7 +1212,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1282,9 +1283,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1639,53 +1637,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="33" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="31" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="31" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1718,16 +1716,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="33" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1752,10 +1750,10 @@
       <c r="B3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1797,61 +1795,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="M1" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="N1" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="O1" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="Q1" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="R1" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="S1" s="33" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1862,55 +1860,55 @@
       <c r="B2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="32">
+      <c r="J2" s="31">
         <v>5</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="M2" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="32" t="s">
+      <c r="N2" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="O2" s="32" t="s">
+      <c r="O2" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="P2" s="32">
+      <c r="P2" s="31">
         <v>640006</v>
       </c>
-      <c r="Q2" s="32" t="s">
+      <c r="Q2" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="R2" s="32" t="s">
+      <c r="R2" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="S2" s="32" t="s">
+      <c r="S2" s="31" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1921,55 +1919,55 @@
       <c r="B3" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="32">
+      <c r="J3" s="31">
         <v>7</v>
       </c>
-      <c r="K3" s="32" t="s">
+      <c r="K3" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="L3" s="32" t="s">
+      <c r="L3" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="M3" s="32" t="s">
+      <c r="M3" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="N3" s="32" t="s">
+      <c r="N3" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="O3" s="32" t="s">
+      <c r="O3" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="P3" s="32">
+      <c r="P3" s="31">
         <v>90069</v>
       </c>
-      <c r="Q3" s="32" t="s">
+      <c r="Q3" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="R3" s="32" t="s">
+      <c r="R3" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="S3" s="32" t="s">
+      <c r="S3" s="31" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2001,80 +1999,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="30" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="32">
+      <c r="H2" s="31">
         <v>9945995011</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="H3" s="32">
+      <c r="H3" s="31">
         <v>9642525696</v>
       </c>
     </row>
@@ -2099,15 +2097,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="16.0909090909091" style="26" customWidth="1"/>
-    <col min="2" max="2" width="12.8181818181818" style="26" customWidth="1"/>
-    <col min="3" max="3" width="85.5454545454545" style="26" customWidth="1"/>
-    <col min="4" max="4" width="19.3636363636364" style="26" customWidth="1"/>
-    <col min="5" max="5" width="18.6363636363636" style="26" customWidth="1"/>
-    <col min="6" max="6" width="20.2727272727273" style="26" customWidth="1"/>
-    <col min="7" max="7" width="15.8181818181818" style="26" customWidth="1"/>
-    <col min="8" max="8" width="23.2727272727273" style="26" customWidth="1"/>
-    <col min="9" max="16384" width="8.72727272727273" style="26"/>
+    <col min="1" max="1" width="16.0909090909091" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.8181818181818" style="2" customWidth="1"/>
+    <col min="3" max="3" width="85.5454545454545" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.3636363636364" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.6363636363636" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.2727272727273" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15.8181818181818" style="2" customWidth="1"/>
+    <col min="8" max="8" width="23.2727272727273" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.72727272727273" style="2"/>
   </cols>
   <sheetData>
     <row r="1" s="25" customFormat="1" spans="1:8">
@@ -2130,27 +2128,27 @@
       <c r="G1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="26" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" ht="72.5" spans="2:8">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="30">
+      <c r="G2" s="29">
         <v>1234567891</v>
       </c>
       <c r="H2" s="24" t="s">

</xml_diff>